<commit_message>
Load TSV/TXT file into Dataframe; Head first 10 lines
</commit_message>
<xml_diff>
--- a/data/Runs.xlsx
+++ b/data/Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wff/dev/py/df/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3B0D1D-4070-454D-85E5-3DBE1B4AA1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC10429-5CB2-CA4F-93DD-28427A828DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,12 +509,13 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="11" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>